<commit_message>
added borders to tables
</commit_message>
<xml_diff>
--- a/Projektdokumentation/Kostenplan.xlsx
+++ b/Projektdokumentation/Kostenplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adpf273313\Aufgaben\Aufgaben 2023\Berufsschule\Abschlussprojekt\School-project\Projektdokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68CCCBE-9F67-44E5-92CE-06CB56D6C57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD316F0-582B-46DC-852E-37E0D7CC826E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t xml:space="preserve">Kostenplan | School Skipper </t>
   </si>
@@ -259,7 +259,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -315,12 +315,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -343,34 +396,49 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -654,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="87" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,30 +744,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="10"/>
-      <c r="L1" s="12" t="s">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="9"/>
+      <c r="L1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="12" t="s">
+      <c r="M1" s="18"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -729,17 +797,17 @@
       <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="10">
         <v>50</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="15" t="s">
+      <c r="P2" s="22"/>
+      <c r="Q2" s="23" t="s">
         <v>22</v>
       </c>
     </row>
@@ -770,22 +838,22 @@
       <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="10">
         <f t="shared" ref="I3:I16" si="1">SUM(F3:H3)</f>
         <v>235.85033783783786</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="19">
         <f>Q8</f>
         <v>0.17925168918918921</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O3" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="8">
+      <c r="P3" s="25"/>
+      <c r="Q3" s="10">
         <f>7.1*2</f>
         <v>14.2</v>
       </c>
@@ -817,15 +885,21 @@
       <c r="H4" s="4">
         <v>0</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="10">
         <f t="shared" si="1"/>
         <v>94.340135135135142</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="L4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="8">
+      <c r="P4" s="25"/>
+      <c r="Q4" s="10">
         <v>700</v>
       </c>
     </row>
@@ -856,15 +930,21 @@
       <c r="H5" s="4">
         <v>0</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="10">
         <f t="shared" si="1"/>
         <v>471.70067567567571</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="L5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="8">
+      <c r="P5" s="25"/>
+      <c r="Q5" s="10">
         <v>20</v>
       </c>
     </row>
@@ -895,15 +975,21 @@
       <c r="H6" s="4">
         <v>0</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="10">
         <f t="shared" si="1"/>
         <v>471.70067567567571</v>
       </c>
-      <c r="O6" s="17" t="s">
+      <c r="L6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="8">
+      <c r="P6" s="25"/>
+      <c r="Q6" s="10">
         <v>42.01</v>
       </c>
     </row>
@@ -934,15 +1020,21 @@
       <c r="H7" s="4">
         <v>0</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="10">
         <f t="shared" si="1"/>
         <v>141.51020270270271</v>
       </c>
-      <c r="O7" s="17" t="s">
+      <c r="L7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="8">
+      <c r="P7" s="25"/>
+      <c r="Q7" s="10">
         <f>142.48*2</f>
         <v>284.95999999999998</v>
       </c>
@@ -974,15 +1066,21 @@
       <c r="H8" s="4">
         <v>0</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="10">
         <f t="shared" si="1"/>
         <v>235.85033783783786</v>
       </c>
-      <c r="O8" s="19" t="s">
+      <c r="L8" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O8" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="P8" s="17"/>
-      <c r="Q8">
+      <c r="P8" s="27"/>
+      <c r="Q8" s="20">
         <f>SUM(Q3:Q7)/F17</f>
         <v>0.17925168918918921</v>
       </c>
@@ -1014,9 +1112,15 @@
       <c r="H9" s="4">
         <v>0</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="10">
         <f t="shared" si="1"/>
         <v>1886.8027027027028</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
@@ -1046,9 +1150,15 @@
       <c r="H10" s="4">
         <v>0</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="10">
         <f t="shared" si="1"/>
         <v>2830.2040540540543</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -1078,9 +1188,15 @@
       <c r="H11" s="4">
         <v>0</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="10">
         <f t="shared" si="1"/>
         <v>235.85033783783786</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="18" x14ac:dyDescent="0.35">
@@ -1110,14 +1226,14 @@
       <c r="H12" s="4">
         <v>0</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="10">
         <f>SUM(F12:H12)</f>
         <v>141.51020270270271</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="12"/>
+      <c r="M12" s="18"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -1146,14 +1262,14 @@
       <c r="H13" s="4">
         <v>0</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="10">
         <f t="shared" si="1"/>
         <v>235.85033783783786</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1174,14 +1290,14 @@
       <c r="H14" s="4">
         <v>0</v>
       </c>
-      <c r="I14" s="20">
+      <c r="I14" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="M14" s="11" t="s">
+      <c r="M14" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1202,14 +1318,14 @@
       <c r="H15" s="4">
         <v>0</v>
       </c>
-      <c r="I15" s="20">
+      <c r="I15" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="M15" s="11" t="s">
+      <c r="M15" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1230,14 +1346,14 @@
       <c r="H16" s="4">
         <v>0</v>
       </c>
-      <c r="I16" s="20">
+      <c r="I16" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="M16" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1270,14 +1386,14 @@
         <f>SUM(H3:H16)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="11">
         <f>SUM(I3:I16)</f>
         <v>6981.170000000001</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="M17" s="17" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new formulas for excel cost calculation and added marketing strategy
</commit_message>
<xml_diff>
--- a/Projektdokumentation/Kostenplan.xlsx
+++ b/Projektdokumentation/Kostenplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adpf273313\Aufgaben\Aufgaben 2023\Berufsschule\Abschlussprojekt\School-project\Projektdokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD316F0-582B-46DC-852E-37E0D7CC826E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D87ADE-1F4D-4167-A978-7406E6CB8A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
   <si>
     <t xml:space="preserve">Kostenplan | School Skipper </t>
   </si>
@@ -104,9 +104,6 @@
     <t>Kostenstelle</t>
   </si>
   <si>
-    <t>pro Monat</t>
-  </si>
-  <si>
     <t>Stromkosten (Alle Mitarbeiter)</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>Mitarbeiterverpflegung (Alle Mitarbeiter)</t>
   </si>
   <si>
-    <t>o2 DSL 250Mbit's Internet</t>
-  </si>
-  <si>
     <t>Büro in Erlangen für zwei Mitarbeiter</t>
   </si>
   <si>
@@ -198,6 +192,21 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>QT-Creator (Alle Mitarbeiter)</t>
+  </si>
+  <si>
+    <t>Kosten für Projektdauer</t>
+  </si>
+  <si>
+    <t>QT-Creator</t>
+  </si>
+  <si>
+    <t>Offizielle Projektdauer (Tage)</t>
+  </si>
+  <si>
+    <t>Telekom 1 Gbit Internet</t>
   </si>
 </sst>
 </file>
@@ -373,7 +382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -400,44 +409,47 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -722,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="87" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,33 +750,34 @@
     <col min="8" max="8" width="15.5546875" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
     <col min="12" max="12" width="36.5546875" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.21875" customWidth="1"/>
     <col min="16" max="16" width="26" customWidth="1"/>
-    <col min="17" max="17" width="11.44140625" customWidth="1"/>
+    <col min="17" max="17" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="19"/>
       <c r="I1" s="9"/>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="18"/>
+      <c r="M1" s="20"/>
       <c r="N1" s="8"/>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="18"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="20"/>
       <c r="R1" s="8"/>
       <c r="S1" s="8"/>
       <c r="T1" s="8"/>
@@ -786,10 +799,10 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
@@ -797,368 +810,379 @@
       <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="12" t="s">
         <v>12</v>
       </c>
       <c r="M2" s="10">
-        <v>50</v>
-      </c>
-      <c r="O2" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="O2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="23" t="s">
-        <v>22</v>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="18" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2">
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="4">
-        <f t="shared" ref="F3:F10" si="0">(C3*D3)*(8*50)</f>
-        <v>200</v>
+        <f>(C3*D3)*(8*M2)</f>
+        <v>100</v>
       </c>
       <c r="G3" s="4">
-        <f>F3*Q8</f>
-        <v>35.850337837837841</v>
+        <f>F3*Q9</f>
+        <v>6.6401351351351359</v>
       </c>
       <c r="H3" s="4">
         <v>0</v>
       </c>
       <c r="I3" s="10">
-        <f t="shared" ref="I3:I16" si="1">SUM(F3:H3)</f>
-        <v>235.85033783783786</v>
-      </c>
-      <c r="L3" s="14" t="s">
+        <f t="shared" ref="I3:I16" si="0">SUM(F3:H3)</f>
+        <v>106.64013513513514</v>
+      </c>
+      <c r="L3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="19">
-        <f>Q8</f>
-        <v>0.17925168918918921</v>
+      <c r="M3" s="16">
+        <f>Q9</f>
+        <v>6.6401351351351362E-2</v>
       </c>
       <c r="O3" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P3" s="25"/>
       <c r="Q3" s="10">
-        <f>7.1*2</f>
-        <v>14.2</v>
+        <f>(7.1*2)/30*M4</f>
+        <v>7.1</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="4">
+        <f>(C4*D4)*(8*M2)</f>
+        <v>100</v>
+      </c>
+      <c r="G4" s="4">
+        <f>F4*Q9</f>
+        <v>6.6401351351351359</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="10">
         <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="G4" s="4">
-        <f>F4*Q8</f>
-        <v>14.340135135135137</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="10">
-        <f t="shared" si="1"/>
-        <v>94.340135135135142</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="M4" s="19" t="s">
-        <v>53</v>
+        <v>106.64013513513514</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="16">
+        <v>15</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P4" s="25"/>
       <c r="Q4" s="10">
-        <v>700</v>
+        <f>700/30*M4</f>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="4">
+        <f>(C5*D5)*(8*M2)</f>
+        <v>1200</v>
+      </c>
+      <c r="G5" s="4">
+        <f>F5*Q9</f>
+        <v>79.68162162162163</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10">
         <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="G5" s="4">
-        <f>F5*Q8</f>
-        <v>71.700675675675683</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0</v>
-      </c>
-      <c r="I5" s="10">
-        <f t="shared" si="1"/>
-        <v>471.70067567567571</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="M5" s="19" t="s">
-        <v>53</v>
+        <v>1279.6816216216216</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="O5" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P5" s="25"/>
       <c r="Q5" s="10">
+        <f>(20*2)/30*M4</f>
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="D6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="4">
+        <f>(C6*D6)*(8*M2)</f>
+        <v>1600</v>
+      </c>
+      <c r="G6" s="4">
+        <f>F6*Q9</f>
+        <v>106.24216216216217</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="10">
         <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="G6" s="4">
-        <f>F6*Q8</f>
-        <v>71.700675675675683</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="10">
-        <f t="shared" si="1"/>
-        <v>471.70067567567571</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>53</v>
+        <v>1706.2421621621622</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="O6" s="24" t="s">
         <v>20</v>
       </c>
       <c r="P6" s="25"/>
       <c r="Q6" s="10">
-        <v>42.01</v>
+        <f>79.95/30*M4</f>
+        <v>39.975000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="2">
-        <v>0.3</v>
+        <v>0.125</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="4">
+        <f>(C7*D7)*(8*M2)</f>
+        <v>100</v>
+      </c>
+      <c r="G7" s="4">
+        <f>F7*Q9</f>
+        <v>6.6401351351351359</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="10">
         <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="G7" s="4">
-        <f>F7*Q8</f>
-        <v>21.510202702702706</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0</v>
-      </c>
-      <c r="I7" s="10">
-        <f t="shared" si="1"/>
-        <v>141.51020270270271</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>53</v>
+        <v>106.64013513513514</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="P7" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="P7" s="29"/>
       <c r="Q7" s="10">
-        <f>142.48*2</f>
-        <v>284.95999999999998</v>
+        <f>4260/360*M4</f>
+        <v>177.5</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="4">
+        <f>(C8*D8)*(8*M2)</f>
+        <v>800</v>
+      </c>
+      <c r="G8" s="4">
+        <f>F8*Q9</f>
+        <v>53.121081081081087</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="10">
         <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="G8" s="4">
-        <f>F8*Q8</f>
-        <v>35.850337837837841</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="10">
-        <f t="shared" si="1"/>
-        <v>235.85033783783786</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="O8" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="20">
-        <f>SUM(Q3:Q7)/F17</f>
-        <v>0.17925168918918921</v>
+        <v>853.12108108108112</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="10">
+        <f>(142.48*2)/30*M4</f>
+        <v>142.47999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
       </c>
       <c r="D9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="4">
+        <f>(C9*D9)*(8*M2)</f>
+        <v>1600</v>
+      </c>
+      <c r="G9" s="4">
+        <f>F9*Q9</f>
+        <v>106.24216216216217</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="10">
         <f t="shared" si="0"/>
-        <v>1600</v>
-      </c>
-      <c r="G9" s="4">
-        <f>F9*Q8</f>
-        <v>286.80270270270273</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="10">
-        <f t="shared" si="1"/>
-        <v>1886.8027027027028</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="M9" s="19" t="s">
-        <v>53</v>
+        <v>1706.2421621621622</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="17">
+        <f>SUM(Q3:Q8)/F17</f>
+        <v>6.6401351351351362E-2</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
       </c>
       <c r="D10" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="4">
+        <f>(C10*D10)*(8*M2)</f>
+        <v>3200</v>
+      </c>
+      <c r="G10" s="4">
+        <f>F10*Q9</f>
+        <v>212.48432432432435</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="10">
         <f t="shared" si="0"/>
-        <v>2400</v>
-      </c>
-      <c r="G10" s="4">
-        <f>F10*Q8</f>
-        <v>430.2040540540541</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0</v>
-      </c>
-      <c r="I10" s="10">
-        <f t="shared" si="1"/>
-        <v>2830.2040540540543</v>
-      </c>
-      <c r="L10" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="M10" s="19" t="s">
-        <v>53</v>
+        <v>3412.4843243243245</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -1172,104 +1196,104 @@
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="4">
-        <f>(C11*D11)*(8*50)</f>
-        <v>200</v>
+        <f>(C11*D11)*(8*M2)</f>
+        <v>800</v>
       </c>
       <c r="G11" s="4">
-        <f>F11*Q8</f>
-        <v>35.850337837837841</v>
+        <f>F11*Q9</f>
+        <v>53.121081081081087</v>
       </c>
       <c r="H11" s="4">
         <v>0</v>
       </c>
       <c r="I11" s="10">
-        <f t="shared" si="1"/>
-        <v>235.85033783783786</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="M11" s="19" t="s">
-        <v>53</v>
+        <f>SUM(F11:H11)</f>
+        <v>853.12108108108112</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
       </c>
       <c r="D12" s="2">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" ref="F12:F16" si="2">(C12*D12)*(8*50)</f>
-        <v>120</v>
+        <f>(C12*D12)*(8*M2)</f>
+        <v>800</v>
       </c>
       <c r="G12" s="4">
-        <f>F12*Q8</f>
-        <v>21.510202702702706</v>
+        <f>F12*Q9</f>
+        <v>53.121081081081087</v>
       </c>
       <c r="H12" s="4">
         <v>0</v>
       </c>
       <c r="I12" s="10">
         <f>SUM(F12:H12)</f>
-        <v>141.51020270270271</v>
-      </c>
-      <c r="L12" s="13" t="s">
+        <v>853.12108108108112</v>
+      </c>
+      <c r="L12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="18"/>
+      <c r="M12" s="20"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
       </c>
       <c r="D13" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="2"/>
-        <v>200</v>
+        <f>(C13*D13)*(8*M2)</f>
+        <v>800</v>
       </c>
       <c r="G13" s="4">
-        <f>F13*Q8</f>
-        <v>35.850337837837841</v>
+        <f>F13*Q9</f>
+        <v>53.121081081081087</v>
       </c>
       <c r="H13" s="4">
         <v>0</v>
       </c>
       <c r="I13" s="10">
-        <f t="shared" si="1"/>
-        <v>235.85033783783786</v>
-      </c>
-      <c r="L13" s="14" t="s">
+        <f t="shared" si="0"/>
+        <v>853.12108108108112</v>
+      </c>
+      <c r="L13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="M13" s="15" t="s">
+      <c r="M13" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1280,24 +1304,24 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="4">
-        <f t="shared" si="2"/>
+        <f>(C14*D14)*(8*M2)</f>
         <v>0</v>
       </c>
       <c r="G14" s="4">
-        <f>F14*Q8</f>
+        <f>F14*Q9</f>
         <v>0</v>
       </c>
       <c r="H14" s="4">
         <v>0</v>
       </c>
       <c r="I14" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="14" t="s">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M14" s="15" t="s">
+      <c r="M14" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1308,24 +1332,24 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="4">
-        <f t="shared" si="2"/>
+        <f>(C15*D15)*(8*M2)</f>
         <v>0</v>
       </c>
       <c r="G15" s="4">
-        <f>F15*Q8</f>
+        <f>F15*Q9</f>
         <v>0</v>
       </c>
       <c r="H15" s="4">
         <v>0</v>
       </c>
       <c r="I15" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="M15" s="15" t="s">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M15" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1336,24 +1360,24 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="4">
-        <f t="shared" si="2"/>
+        <f>(C16*D16)*(8*M2)</f>
         <v>0</v>
       </c>
       <c r="G16" s="4">
-        <f>F16*Q8</f>
+        <f>F16*Q9</f>
         <v>0</v>
       </c>
       <c r="H16" s="4">
         <v>0</v>
       </c>
       <c r="I16" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="M16" s="15" t="s">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="M16" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1362,25 +1386,25 @@
         <v>10</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D17" s="6">
-        <f>SUM(D3:D16)</f>
-        <v>9.8000000000000007</v>
+        <f>SUMPRODUCT(C3:C13, D3:D13)</f>
+        <v>13.875</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F17" s="7">
         <f>SUM(F3:F16)</f>
-        <v>5920</v>
+        <v>11100</v>
       </c>
       <c r="G17" s="7">
         <f>SUM(G3:G16)</f>
-        <v>1061.17</v>
+        <v>737.05500000000018</v>
       </c>
       <c r="H17" s="7">
         <f>SUM(H3:H16)</f>
@@ -1388,12 +1412,12 @@
       </c>
       <c r="I17" s="11">
         <f>SUM(I3:I16)</f>
-        <v>6981.170000000001</v>
-      </c>
-      <c r="L17" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="M17" s="17" t="s">
+        <v>11837.054999999998</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1406,6 +1430,12 @@
       <c r="F18" s="4"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
+      <c r="L18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
@@ -1478,7 +1508,7 @@
       <c r="H25" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="L12:M12"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="L1:M1"/>
@@ -1488,16 +1518,17 @@
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
     <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A11" r:id="rId1" xr:uid="{26567021-B104-4E46-A346-D8B387CF36F6}"/>
     <hyperlink ref="M13" r:id="rId2" location=":~:text=auf%20dich%20zukommen%20%E2%80%A6-,Was%20kostet%20ein%20Software%2DEntwickler%20pro%20Stunde%3F,40%20%E2%82%AC%20%2D%2060%20%E2%82%AC%20an." xr:uid="{D15B92D6-22C0-4530-A201-034F083F3042}"/>
     <hyperlink ref="M14" r:id="rId3" xr:uid="{3A5990A4-01DE-424A-8910-CF04E39CA364}"/>
     <hyperlink ref="M15" r:id="rId4" xr:uid="{406E886F-0BEA-4C96-A657-AF950975B4D7}"/>
-    <hyperlink ref="M16" r:id="rId5" location="/" xr:uid="{863AB92B-32C7-45C2-B3D1-5F7E306DACF1}"/>
-    <hyperlink ref="M17" r:id="rId6" xr:uid="{C78F1DAE-DA5A-44FC-AA66-2B39D8A13893}"/>
+    <hyperlink ref="M17" r:id="rId5" location="/" xr:uid="{863AB92B-32C7-45C2-B3D1-5F7E306DACF1}"/>
+    <hyperlink ref="M18" r:id="rId6" xr:uid="{C78F1DAE-DA5A-44FC-AA66-2B39D8A13893}"/>
     <hyperlink ref="A12" r:id="rId7" xr:uid="{C7D6FC5E-271C-4635-A436-E96B5CF174A5}"/>
     <hyperlink ref="A8" r:id="rId8" xr:uid="{B3FE82B5-C39D-4A18-B4D2-3D46742241CC}"/>
     <hyperlink ref="A7" r:id="rId9" xr:uid="{18BEC918-5002-4B09-B8AB-24D65920DB7F}"/>
@@ -1506,6 +1537,7 @@
     <hyperlink ref="A13" r:id="rId12" xr:uid="{005E8D96-7C76-4804-A6D2-D08004F8868E}"/>
     <hyperlink ref="A3" r:id="rId13" xr:uid="{2C55C562-A497-4336-A502-387FA561A961}"/>
     <hyperlink ref="A5" r:id="rId14" xr:uid="{2EE723AE-0605-45EB-A1E5-4060EE958202}"/>
+    <hyperlink ref="M16" r:id="rId15" xr:uid="{B5377B6A-31A0-4973-8C3B-28E0608AF03B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>